<commit_message>
add file for data extraction from WMS and file to divide large data file into smaller one
</commit_message>
<xml_diff>
--- a/Documents/Work Log.xlsx
+++ b/Documents/Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yunyu\Desktop\s\19s2\COMP8715\Project\energy_storage_rights-master\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF2D297-86D6-49A1-8368-1FA3E17D5E16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582D49BB-53BF-456D-BF0A-6F35EEFDA18F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{89E77A1C-D209-4B2D-90C1-A1F1CBCAECAC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -556,6 +556,152 @@
   </si>
   <si>
     <t>1.5 Hour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 Hour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove GDAL, divide large data file into smaller data files</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update SOW with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Weiwei</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update SOW with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yuanxin</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Explore how to extract data from a WMS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trying to implement webserver with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Peilin</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trying to implement webserver with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dawei</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Research on maintainence cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Explore how to extract data from a WMS. Work together with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yunyuan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Explore how to extract data from a WMS. Work together with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Daoyu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1555,8 +1701,8 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13:K13"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1585,7 +1731,7 @@
       </c>
       <c r="J1" s="40">
         <f>SUM(D4:D30)</f>
-        <v>18.5</v>
+        <v>22.5</v>
       </c>
       <c r="L1" s="34"/>
     </row>
@@ -1962,35 +2108,69 @@
       <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
+      <c r="A14" s="17">
+        <v>43692</v>
+      </c>
+      <c r="B14" s="18">
+        <v>0.5625</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="D14" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="28"/>
+        <v>3</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>64</v>
+      </c>
       <c r="L14" s="31"/>
       <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
+      <c r="A15" s="17">
+        <v>43692</v>
+      </c>
+      <c r="B15" s="18">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>35</v>
+      </c>
       <c r="D15" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="28"/>

</xml_diff>

<commit_message>
update 2 jupyter file
</commit_message>
<xml_diff>
--- a/Documents/Work Log.xlsx
+++ b/Documents/Work Log.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yunyu\Desktop\s\19s2\COMP8715\Project\energy_storage_rights-master\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582D49BB-53BF-456D-BF0A-6F35EEFDA18F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851916F4-6063-418D-B99A-56C701068D6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{89E77A1C-D209-4B2D-90C1-A1F1CBCAECAC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -488,24 +488,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">reorganize Github directory. Work with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Yuanxin</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Finished editing SOW and reorganize GitHub
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -643,10 +625,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Research on maintainence cost</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Explore how to extract data from a WMS. Work together with </t>
     </r>
@@ -702,6 +680,202 @@
       </rPr>
       <t>.</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Develop algorithm to compress data.
+Develop algorithm to divide data into smaller files.
+Distance to transmission line data from WMS is extracted, Continue to try to extract Pumped Hydro data. Work together with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Daoyu</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Working with Heroku. Work together with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dawei</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Working with Heroku. Work together with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Peilin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 Hour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Research on maintainence cost for solar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Research on maintainence cost for wind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Research on cost for transmission line. Work together with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yufei</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Research on cost for transmission line. Work together with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Weiwei</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Distance to transmission line data from WMS is extracted, Continue to try to extract Pumped Hydro data. Work together with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Yunyuan</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update trelloe, Github</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meet with client, MEETING MINUTES 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meet with client, MEETING MINUTES 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meet with client, MEETING MINUTES 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meet with client, MEETING MINUTES 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up bootstrap environment,  Design a new navigation bar and side bar without functions.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modified statement of work. Readjut deliverable base on the client feedback.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trying to implement webserver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Explore how to extract data from a WMS.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue refine statement of work.Review information on other section in SOW. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6 Hour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1。5 Hour</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -714,7 +888,7 @@
     <numFmt numFmtId="177" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -757,8 +931,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="14"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
@@ -786,7 +976,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -829,21 +1019,6 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1078,19 +1253,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1181,17 +1343,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1218,80 +1369,148 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1300,12 +1519,18 @@
     <xf numFmtId="177" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1318,44 +1543,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1363,26 +1567,53 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="6" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1698,797 +1929,948 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4BC723-20AC-4C13-97D4-E732BE13825D}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.5546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="24" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="29.77734375" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5546875" style="23" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="23" hidden="1" customWidth="1"/>
     <col min="5" max="11" width="27.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="42.44140625" style="33" customWidth="1"/>
+    <col min="12" max="12" width="42.44140625" style="32" customWidth="1"/>
     <col min="13" max="13" width="32.77734375" style="2" customWidth="1"/>
     <col min="14" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="13" customFormat="1" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:13" s="12" customFormat="1" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="I1" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="40">
-        <f>SUM(D4:D30)</f>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="I1" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="55">
+        <f>SUM(D4:D34)</f>
+        <v>30.5</v>
+      </c>
+      <c r="L1" s="33"/>
+    </row>
+    <row r="2" spans="1:13" s="25" customFormat="1" ht="44.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="44"/>
+      <c r="E2" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="25" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="45"/>
+      <c r="E3" s="47">
+        <f>Worksheet!$J$1-SUMIF(Worksheet!E$4:E$104,"",Worksheet!$D$4:$D$104)</f>
+        <v>21.5</v>
+      </c>
+      <c r="F3" s="47">
+        <f>Worksheet!$J$1-SUMIF(Worksheet!F$4:F$104,"",Worksheet!$D$4:$D$104)</f>
+        <v>20.5</v>
+      </c>
+      <c r="G3" s="47">
+        <f>Worksheet!$J$1-SUMIF(Worksheet!G$4:G$104,"",Worksheet!$D$4:$D$104)</f>
+        <v>20.5</v>
+      </c>
+      <c r="H3" s="47">
+        <f>Worksheet!$J$1-SUMIF(Worksheet!H$4:H$104,"",Worksheet!$D$4:$D$104)</f>
         <v>22.5</v>
       </c>
-      <c r="L1" s="34"/>
-    </row>
-    <row r="2" spans="1:13" s="26" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="26" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="52"/>
+      <c r="I3" s="47">
+        <f>Worksheet!$J$1-SUMIF(Worksheet!I$4:I$104,"",Worksheet!$D$4:$D$104)</f>
+        <v>20.5</v>
+      </c>
+      <c r="J3" s="47">
+        <f>Worksheet!$J$1-SUMIF(Worksheet!J$4:J$104,"",Worksheet!$D$4:$D$104)</f>
+        <v>21</v>
+      </c>
+      <c r="K3" s="47">
+        <f>Worksheet!$J$1-SUMIF(Worksheet!K$4:K$104,"",Worksheet!$D$4:$D$104)</f>
+        <v>21.5</v>
+      </c>
       <c r="L3" s="43"/>
       <c r="M3" s="43"/>
     </row>
     <row r="4" spans="1:13" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14">
+      <c r="A4" s="13">
         <v>43607</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="34">
         <f>IF(ISNUMBER(SEARCH("Hour",C4)),_xlfn.NUMBERVALUE(LEFT(C4,SEARCH("Hour",C4)-2)),IF(ISNUMBER(SEARCH("Min",C4)),_xlfn.NUMBERVALUE(LEFT(C4,SEARCH("Min",C4)-2)),0)/60)</f>
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="30" t="s">
+      <c r="K4" s="26"/>
+      <c r="L4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
+    <row r="5" spans="1:13" ht="117.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
         <v>43678</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="35">
-        <f t="shared" ref="D5:D30" si="0">IF(ISNUMBER(SEARCH("Hour",C5)),_xlfn.NUMBERVALUE(LEFT(C5,SEARCH("Hour",C5)-2)),IF(ISNUMBER(SEARCH("Min",C5)),_xlfn.NUMBERVALUE(LEFT(C5,SEARCH("Min",C5)-2)),0)/60)</f>
+      <c r="D5" s="34">
+        <f t="shared" ref="D5:D34" si="0">IF(ISNUMBER(SEARCH("Hour",C5)),_xlfn.NUMBERVALUE(LEFT(C5,SEARCH("Hour",C5)-2)),IF(ISNUMBER(SEARCH("Min",C5)),_xlfn.NUMBERVALUE(LEFT(C5,SEARCH("Min",C5)-2)),0)/60)</f>
         <v>3</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="31" t="s">
+      <c r="K5" s="27"/>
+      <c r="L5" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="9"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" ht="118.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>43678</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="34">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8" t="s">
+      <c r="H6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="28" t="s">
+      <c r="J6" s="7"/>
+      <c r="K6" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="31" t="s">
+      <c r="L6" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="9"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" ht="103.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>43681</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <v>0.625</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="34">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="28" t="s">
+      <c r="I7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="L7" s="31" t="s">
+      <c r="L7" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="9"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>43681</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <v>0.6875</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="34">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="E8" s="50" t="s">
+      <c r="E8" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="9"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
+      <c r="A9" s="16">
         <v>43681</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="17">
         <v>0.69791666666666663</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="34">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="E9" s="50" t="s">
+      <c r="E9" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="9"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" ht="83.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17">
+      <c r="A10" s="16">
         <v>43681</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="34">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="L10" s="31" t="s">
+      <c r="L10" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="9"/>
+      <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
+      <c r="A11" s="16">
         <v>43681</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>0.75</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="34">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6"/>
+      <c r="F11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L11" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="M11" s="9"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" ht="111" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17">
+      <c r="A12" s="16">
         <v>43681</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="34">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="J12" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="28"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="9"/>
+      <c r="K12" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="30"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
+      <c r="A13" s="16">
         <v>43683</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="17">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="35">
+      <c r="C13" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="34">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>43683</v>
+      </c>
+      <c r="B14" s="17">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>43691</v>
+      </c>
+      <c r="B15" s="17">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
+      <c r="D15" s="34"/>
+      <c r="E15" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
         <v>43692</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B16" s="17">
         <v>0.5625</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="35">
+      <c r="C16" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="34">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="J16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="L14" s="31"/>
-      <c r="M14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
+      <c r="K16" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="30"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
         <v>43692</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B17" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C17" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D17" s="34">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" s="30"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" ht="62.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>43692</v>
+      </c>
+      <c r="B18" s="17">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="34">
+        <f>IF(ISNUMBER(SEARCH("Hour",C18)),_xlfn.NUMBERVALUE(LEFT(C18,SEARCH("Hour",C18)-2)),IF(ISNUMBER(SEARCH("Min",C18)),_xlfn.NUMBERVALUE(LEFT(C18,SEARCH("Min",C18)-2)),0)/60)</f>
+        <v>2</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="L18" s="30"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>43698</v>
+      </c>
+      <c r="B19" s="17">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>43700</v>
+      </c>
+      <c r="B20" s="17">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" ht="124.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>43702</v>
+      </c>
+      <c r="B21" s="17">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="34">
+        <f>IF(ISNUMBER(SEARCH("Hour",C21)),_xlfn.NUMBERVALUE(LEFT(C21,SEARCH("Hour",C21)-2)),IF(ISNUMBER(SEARCH("Min",C21)),_xlfn.NUMBERVALUE(LEFT(C21,SEARCH("Min",C21)-2)),0)/60)</f>
+        <v>6</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="35">
+      <c r="J21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="L21" s="30"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="35">
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="9"/>
-    </row>
-    <row r="18" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="35">
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="9"/>
-    </row>
-    <row r="19" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="35">
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="9"/>
-    </row>
-    <row r="20" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="35">
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="35">
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="9"/>
-    </row>
-    <row r="22" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="35">
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="8"/>
+    </row>
+    <row r="28" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="9"/>
-    </row>
-    <row r="23" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="35">
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="8"/>
+    </row>
+    <row r="29" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="9"/>
-    </row>
-    <row r="24" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="35">
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="16"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="9"/>
-    </row>
-    <row r="25" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="35">
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="9"/>
-    </row>
-    <row r="26" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="35">
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="8"/>
+    </row>
+    <row r="32" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="16"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="9"/>
-    </row>
-    <row r="27" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="35">
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="9"/>
-    </row>
-    <row r="28" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="35">
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="30"/>
+      <c r="M33" s="8"/>
+    </row>
+    <row r="34" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="9"/>
-    </row>
-    <row r="29" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="9"/>
-    </row>
-    <row r="30" spans="1:13" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="12"/>
-    </row>
-    <row r="31" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="38"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D32" s="38"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="38"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="38"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="38"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="38"/>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="38"/>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="38"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="11"/>
+    </row>
+    <row r="35" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="35"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D36" s="35"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D37" s="35"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D38" s="35"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D39" s="35"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D40" s="35"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D41" s="35"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D42" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="8">
+    <mergeCell ref="E20:K20"/>
+    <mergeCell ref="E14:K14"/>
+    <mergeCell ref="E15:K15"/>
+    <mergeCell ref="E19:K19"/>
     <mergeCell ref="E13:K13"/>
-    <mergeCell ref="M2:M3"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
     <mergeCell ref="E9:K9"/>
     <mergeCell ref="E8:K8"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>